<commit_message>
chỉnh lại validate ThoiHan,validate TenChungChi, Hiện message
Chỉnh sửa Chứng chỉ (Certificate) và Bằng cấp-giấy chứng nhận (Diploma)
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/TCLD/Certificate/Chứng chỉ của cả công ty.xlsx
+++ b/QUANGHANH2/excel/TCLD/Certificate/Chứng chỉ của cả công ty.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,23 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Tên chứng chỉ</t>
+  </si>
+  <si>
+    <t>Thời hạn (tháng)</t>
+  </si>
+  <si>
+    <t>Kiểu chứng chỉ</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +42,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +77,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -114,7 +170,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +205,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +387,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chỉnh format excel, thêm message cho tìm kiếm
Chỉnh sửa format excel của Certificate( Chứng chỉ) ,Diploma(Bằng cấp và giấy chứng nhận).
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/TCLD/Certificate/Chứng chỉ của cả công ty.xlsx
+++ b/QUANGHANH2/excel/TCLD/Certificate/Chứng chỉ của cả công ty.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Tên chứng chỉ</t>
   </si>
@@ -29,12 +29,18 @@
   <si>
     <t>Kiểu chứng chỉ</t>
   </si>
+  <si>
+    <t>Bảng danh sách chứng chỉ công ty</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,8 +60,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -68,8 +86,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -78,16 +102,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -96,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -104,7 +135,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -387,32 +424,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="39.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="25.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>